<commit_message>
este fue el cambio de la obra 4
</commit_message>
<xml_diff>
--- a/Nuevo Hoja de cálculo de Microsoft Exce22222222222l.xlsx
+++ b/Nuevo Hoja de cálculo de Microsoft Exce22222222222l.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e_dav\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5828a9b8adc7f405/Escritorio/Git/Prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE7BFD8-A4C0-4F3A-B855-2EF132F22058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{5BE7BFD8-A4C0-4F3A-B855-2EF132F22058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{537A973A-6542-418F-957E-A9606E1C9136}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="5">
   <si>
     <t>a</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -354,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -378,7 +381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -386,12 +389,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -399,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -407,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -415,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -423,35 +426,66 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>